<commit_message>
Pushing highlighted voice lines.
</commit_message>
<xml_diff>
--- a/Narrative/Devan's Voice Lines/Codes with Subtitles.xlsx
+++ b/Narrative/Devan's Voice Lines/Codes with Subtitles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DBG17\OneDrive\Desktop\GIT HUB REPOS\GameDesign\FinalGame\Narrative\Devan's Voice Lines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98FA012F-8DCC-41BC-8A72-BA03D262930D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0BACFD-3DBB-4E05-A205-4ECD5BEB7776}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14430" yWindow="480" windowWidth="21600" windowHeight="11505" xr2:uid="{3594FC1F-0F3D-4291-A0C4-59649E3FC225}"/>
+    <workbookView xWindow="8805" yWindow="120" windowWidth="21600" windowHeight="11505" xr2:uid="{3594FC1F-0F3D-4291-A0C4-59649E3FC225}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="96">
   <si>
     <t>001</t>
   </si>
@@ -304,6 +304,21 @@
   </si>
   <si>
     <t>The spare switch? Must be by those spares in the workshop.</t>
+  </si>
+  <si>
+    <t>This is my home… they can’t just take this place away from me</t>
+  </si>
+  <si>
+    <t>He should understand… he grew up here with us. I can’t just leave, not like he did.</t>
+  </si>
+  <si>
+    <t>Alex used to be stuck in these books of hers for hours, she was always the smart one.</t>
+  </si>
+  <si>
+    <t>That tool head is loose on that hoe, I should wedge some wood in there later…</t>
+  </si>
+  <si>
+    <t>Thar she is… the beauty. I remember taking Nichola out on that old boat. Taught him to fish like my paps taught me.</t>
   </si>
 </sst>
 </file>
@@ -334,7 +349,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -344,6 +359,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -375,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -391,6 +418,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -707,439 +738,461 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF1651A-87F8-47B3-B03B-022E67FAA57F}">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="62.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="102.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="62.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="102.5703125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="C28" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="C29" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="C30" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="C32" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="C33" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="C34" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="C35" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="C36" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="C37" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="C38" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="C39" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="C40" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="7"/>
+      <c r="B41" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="C41" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+      <c r="D41" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="7"/>
+      <c r="B42" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="C42" s="4" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+      <c r="D42" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="C43" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="C44" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="7"/>
+      <c r="B45" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="C45" s="4" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+      <c r="D45" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="7"/>
+      <c r="B46" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="C46" s="4" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+      <c r="D46" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="7"/>
+      <c r="B47" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="C47" s="4" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+      <c r="D47" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="C48" s="4" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1148,7 +1201,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A2:A26 A49:A1048576" numberStoredAsText="1"/>
+    <ignoredError sqref="B2:B26 B49:B1048576 B27:B48" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ordering the Voice Lines into files.
</commit_message>
<xml_diff>
--- a/Narrative/Devan's Voice Lines/Codes with Subtitles.xlsx
+++ b/Narrative/Devan's Voice Lines/Codes with Subtitles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DBG17\OneDrive\Desktop\GIT HUB REPOS\GameDesign\FinalGame\Narrative\Devan's Voice Lines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0BACFD-3DBB-4E05-A205-4ECD5BEB7776}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13985864-73E0-4E86-83EA-8CE0938F80E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8805" yWindow="120" windowWidth="21600" windowHeight="11505" xr2:uid="{3594FC1F-0F3D-4291-A0C4-59649E3FC225}"/>
+    <workbookView xWindow="3885" yWindow="720" windowWidth="21600" windowHeight="11505" xr2:uid="{3594FC1F-0F3D-4291-A0C4-59649E3FC225}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="96">
   <si>
     <t>001</t>
   </si>
@@ -740,7 +740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF1651A-87F8-47B3-B03B-022E67FAA57F}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>